<commit_message>
Added licor QC check for negative concentrations
</commit_message>
<xml_diff>
--- a/metadata/trh_profile_metadata.xlsx
+++ b/metadata/trh_profile_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42148975-B897-F048-81BF-7A6E95C1A880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49B0AF2-4F9B-2543-A740-D05A18230228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31300" yWindow="-1420" windowWidth="34520" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,9 +232,6 @@
     <t xml:space="preserve">Point measurements of temperature/ humidity from HMP155 sensors at four levels on the Summit Station met tower. </t>
   </si>
   <si>
-    <t>CF-1.6,</t>
-  </si>
-  <si>
     <t>ace-tower: T/RH sensors 1-4</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Acknowledgement of the following grants is required: NSFGE Grant Award number: 1801318, NERC Grant Award number NE/S00906X/1</t>
+  </si>
+  <si>
+    <t>CF-1.6</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -910,7 +910,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -970,7 +970,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>

</xml_diff>